<commit_message>
included multifile support via file split
</commit_message>
<xml_diff>
--- a/tests/reference_files/lab_journal.xlsx
+++ b/tests/reference_files/lab_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="132">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -70,7 +70,7 @@
     <t xml:space="preserve">False</t>
   </si>
   <si>
-    <t xml:space="preserve">Nanosurf Easysurf</t>
+    <t xml:space="preserve">Nanosurf Easysurf STM image</t>
   </si>
   <si>
     <t xml:space="preserve">Au_a</t>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">Au(111)</t>
   </si>
   <si>
-    <t xml:space="preserve">XPS self-written software E20</t>
+    <t xml:space="preserve">XPS software E20</t>
   </si>
   <si>
     <t xml:space="preserve">MK19_autoclave</t>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">hopg</t>
   </si>
   <si>
-    <t xml:space="preserve">Renishaw Raman Image</t>
+    <t xml:space="preserve">Optical Microscopy Image</t>
   </si>
   <si>
     <t xml:space="preserve">CV_162437_ 1</t>
@@ -217,7 +217,7 @@
     <t xml:space="preserve">sem</t>
   </si>
   <si>
-    <t xml:space="preserve">FEI SEM IMAGE</t>
+    <t xml:space="preserve">FEI SEM Image</t>
   </si>
   <si>
     <t xml:space="preserve">xps_phi</t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">Park AFM</t>
   </si>
   <si>
-    <t xml:space="preserve">GrRu_RT</t>
+    <t xml:space="preserve">GrRu_RT_1</t>
   </si>
   <si>
     <t xml:space="preserve">etched</t>
@@ -247,7 +247,175 @@
     <t xml:space="preserve">GrRu</t>
   </si>
   <si>
-    <t xml:space="preserve">Specs STM</t>
+    <t xml:space="preserve">Specs STM Multifile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GrRu_RT_57</t>
   </si>
 </sst>
 </file>
@@ -391,26 +559,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="N68" activeCellId="0" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="38.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,6 +1002,1126 @@
         <v>74</v>
       </c>
       <c r="L17" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L46" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L47" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L51" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L52" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L57" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L58" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L59" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L60" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L61" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L62" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L65" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L67" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L68" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L69" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L70" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L71" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L72" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L73" s="0" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced exec with dict
</commit_message>
<xml_diff>
--- a/tests/reference_files/lab_journal.xlsx
+++ b/tests/reference_files/lab_journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="134">
   <si>
     <t xml:space="preserve">day</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">remark</t>
   </si>
   <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
     <t xml:space="preserve">stm</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nanosurf Easysurf STM image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">271</t>
   </si>
   <si>
     <t xml:space="preserve">Au_a</t>
@@ -562,9 +568,9 @@
   <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N68" activeCellId="0" sqref="N68"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -623,46 +629,46 @@
       <c r="A2" s="1" t="n">
         <v>43556</v>
       </c>
-      <c r="B2" s="6" t="n">
-        <v>37</v>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>43556</v>
       </c>
-      <c r="B3" s="6" t="n">
-        <v>271</v>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,63 +676,63 @@
         <v>43556</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>43602</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I5" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -737,13 +743,13 @@
         <v>448</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -751,16 +757,16 @@
         <v>43821</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,45 +774,45 @@
         <v>43821</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>43852</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,28 +820,28 @@
         <v>43852</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="G10" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,31 +849,31 @@
         <v>43854</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -875,31 +881,31 @@
         <v>43854</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>53</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,31 +913,31 @@
         <v>43858</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,16 +945,16 @@
         <v>43858</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,16 +962,16 @@
         <v>43876</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,16 +979,16 @@
         <v>43878</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -990,19 +996,19 @@
         <v>44248</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1010,19 +1016,19 @@
         <v>44248</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,19 +1036,19 @@
         <v>44248</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,19 +1056,19 @@
         <v>44248</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,19 +1076,19 @@
         <v>44248</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,19 +1096,19 @@
         <v>44248</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,19 +1116,19 @@
         <v>44248</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1130,19 +1136,19 @@
         <v>44248</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,19 +1156,19 @@
         <v>44248</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1170,19 +1176,19 @@
         <v>44248</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,19 +1196,19 @@
         <v>44248</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,19 +1216,19 @@
         <v>44248</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,19 +1236,19 @@
         <v>44248</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1250,19 +1256,19 @@
         <v>44248</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,19 +1276,19 @@
         <v>44248</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,19 +1296,19 @@
         <v>44248</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,19 +1316,19 @@
         <v>44248</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1330,19 +1336,19 @@
         <v>44248</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,19 +1356,19 @@
         <v>44248</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,19 +1376,19 @@
         <v>44248</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1390,19 +1396,19 @@
         <v>44248</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,19 +1416,19 @@
         <v>44248</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,19 +1436,19 @@
         <v>44248</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1450,19 +1456,19 @@
         <v>44248</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,19 +1476,19 @@
         <v>44248</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L41" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,19 +1496,19 @@
         <v>44248</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,19 +1516,19 @@
         <v>44248</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,19 +1536,19 @@
         <v>44248</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,19 +1556,19 @@
         <v>44248</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L45" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,19 +1576,19 @@
         <v>44248</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L46" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,19 +1596,19 @@
         <v>44248</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,19 +1616,19 @@
         <v>44248</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L48" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,19 +1636,19 @@
         <v>44248</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L49" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,19 +1656,19 @@
         <v>44248</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L50" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,19 +1676,19 @@
         <v>44248</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L51" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,19 +1696,19 @@
         <v>44248</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L52" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,19 +1716,19 @@
         <v>44248</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L53" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1730,19 +1736,19 @@
         <v>44248</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L54" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,19 +1756,19 @@
         <v>44248</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L55" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,19 +1776,19 @@
         <v>44248</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L56" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,19 +1796,19 @@
         <v>44248</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L57" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,19 +1816,19 @@
         <v>44248</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,19 +1836,19 @@
         <v>44248</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,19 +1856,19 @@
         <v>44248</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,19 +1876,19 @@
         <v>44248</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L61" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,19 +1896,19 @@
         <v>44248</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L62" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,19 +1916,19 @@
         <v>44248</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L63" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,19 +1936,19 @@
         <v>44248</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L64" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1950,19 +1956,19 @@
         <v>44248</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L65" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,19 +1976,19 @@
         <v>44248</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L66" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,19 +1996,19 @@
         <v>44248</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L67" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,19 +2016,19 @@
         <v>44248</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L68" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,19 +2036,19 @@
         <v>44248</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L69" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,19 +2056,19 @@
         <v>44248</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L70" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2070,19 +2076,19 @@
         <v>44248</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L71" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,19 +2096,19 @@
         <v>44248</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L72" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,19 +2116,19 @@
         <v>44248</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L73" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>